<commit_message>
auto commit rep - metro
</commit_message>
<xml_diff>
--- a/Dataset/Данные станций и линий метро.xlsx
+++ b/Dataset/Данные станций и линий метро.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brazilec22/Documents/LCT_HACK/Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEBA6A5-F495-0944-95C0-3E523972A043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8129230C-F0FF-7E49-A06B-F9FF67ABCDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Список станций" sheetId="1" r:id="rId1"/>
@@ -16865,7 +16865,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>